<commit_message>
update contoh master barang bertingkat
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangHargaBertingkat.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangHargaBertingkat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42897BB5-4F34-49E5-B1B4-66F6921783D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C0C271-9A4D-4887-ACC6-77D968BDCEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -563,25 +563,25 @@
         <v>15</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>33000</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>31000</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>28000</v>
       </c>
       <c r="L2">
         <v>7916248854</v>

</xml_diff>

<commit_message>
update master barang bertingkat 3 item, update master barang multi satuan 4 satuan
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangHargaBertingkat.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangHargaBertingkat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C0C271-9A4D-4887-ACC6-77D968BDCEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD204AFA-9EA3-4171-8506-BC5E84472587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>NAMABARANG</t>
   </si>
@@ -80,6 +80,12 @@
   </si>
   <si>
     <t>SUBKATEGORI</t>
+  </si>
+  <si>
+    <t>JML3</t>
+  </si>
+  <si>
+    <t>HARGAJUAL3</t>
   </si>
 </sst>
 </file>
@@ -93,7 +99,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +151,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,7 +190,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -204,6 +216,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -481,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -500,12 +515,14 @@
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,17 +556,23 @@
       <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -575,21 +598,27 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>31000</v>
+        <v>33000</v>
       </c>
       <c r="J2">
         <v>50</v>
       </c>
       <c r="K2">
+        <v>31000</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
+      </c>
+      <c r="M2">
         <v>28000</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>7916248854</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update master barang bertingkaT
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterBarangHargaBertingkat.xlsx
+++ b/ImportExport/ExcelFiles/MasterBarangHargaBertingkat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KERJA\AXATA\AxataPOSFilesResources\AxataPOSFilesResources\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD204AFA-9EA3-4171-8506-BC5E84472587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6451A3-359E-4A7F-8F7C-68B41CD351FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -598,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>33000</v>
+        <v>32000</v>
       </c>
       <c r="J2">
         <v>50</v>

</xml_diff>